<commit_message>
Printing logic good for extraction
</commit_message>
<xml_diff>
--- a/scrape_targets.xlsx
+++ b/scrape_targets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\PythonProjects\ExcelExtractorPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8D12F1-F4E0-42B8-8568-97E6F3C05455}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2FF86C-5AD3-4D43-8770-E7B7AC4F8944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="5540" windowWidth="28800" windowHeight="15460" xr2:uid="{518FEAFD-939C-4A7D-A483-F0BB88014974}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15460" xr2:uid="{518FEAFD-939C-4A7D-A483-F0BB88014974}"/>
   </bookViews>
   <sheets>
     <sheet name="target_data" sheetId="1" r:id="rId1"/>
@@ -40,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>sql_table</t>
   </si>
@@ -169,9 +191,6 @@
     <t>The cell value IF and ONLY IF it's a specific cell</t>
   </si>
   <si>
-    <t>The starting cell IF AND ONLY IF the target is a range</t>
-  </si>
-  <si>
     <t>As range_start but end cell</t>
   </si>
   <si>
@@ -278,13 +297,30 @@
   </si>
   <si>
     <t>Try to keep cells to their own tables and ranges to their own tables. If you have a table where one column is 'Country Name' and it = 'England' and you try to include a range in the same table, say 'Year' which runs from 1900 to 2000, then you will end up with the 'Country Name' column containing 100x instances of 'England'. This is very data inefficient and if you begin working with hundreds or thousands of mixed cell/range tables then you will soon get into millions of rows/columns of data where there should only be thousands (think: GB of data vs MB or even KB)</t>
+  </si>
+  <si>
+    <t>range_target</t>
+  </si>
+  <si>
+    <t>The starting cell IF AND ONLY IF the target is a range. Range start/end must be same row/column.
+Examples:
+BAD: A1:Z10 (cross rows and columns)
+GOOD: A1:A10 (same column)
+GOOD A1:Z1 (same row)
+Basically: If the range is the same row, or same column then it's fine. If the range crosses multiple rows or multiple columns then it won't work. These should be approached as separate rows/columns.</t>
+  </si>
+  <si>
+    <t>is_range_valid</t>
+  </si>
+  <si>
+    <t>range_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +330,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,15 +377,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="18">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -382,10 +430,76 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -401,9 +515,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{463491B0-F0FB-4A54-A8DF-FE4522A53DC6}" name="Table1" displayName="Table1" ref="A1:I15" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="A1:I15" xr:uid="{1CBFAB26-4B89-4259-9A52-23CEBACB033B}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{463491B0-F0FB-4A54-A8DF-FE4522A53DC6}" name="Table1" displayName="Table1" ref="A1:L15" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:L15" xr:uid="{1CBFAB26-4B89-4259-9A52-23CEBACB033B}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{A93C40C7-C2F4-4A55-81DC-2E3E4884ACA4}" name="source_sheet"/>
     <tableColumn id="2" xr3:uid="{F7A916CE-56BF-450D-8D09-4C0D3640E4FB}" name="sql_table"/>
     <tableColumn id="3" xr3:uid="{5E08581E-A626-41E4-A3A6-E7092DE71F3F}" name="column_name"/>
@@ -411,7 +525,16 @@
     <tableColumn id="5" xr3:uid="{3D4629AB-F2BC-47C5-8349-7E109F964BFA}" name="cell_position"/>
     <tableColumn id="6" xr3:uid="{54F89EEC-33E3-407A-A390-2297247EA74B}" name="range_data_start"/>
     <tableColumn id="7" xr3:uid="{F060C16F-F16D-4308-A0EB-522EA932101E}" name="range_data_end"/>
-    <tableColumn id="8" xr3:uid="{00410D75-8C08-440A-93CF-CB2178D50F9C}" name="pandas_data_type"/>
+    <tableColumn id="13" xr3:uid="{F5983EFB-EE48-4D35-9D9F-1E17636F31B3}" name="pandas_data_type"/>
+    <tableColumn id="10" xr3:uid="{565D067D-9EC2-44EE-B453-12007052D0AC}" name="range_target" dataDxfId="14">
+      <calculatedColumnFormula>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{262BC145-114C-40E5-A310-C6C9AB7BE343}" name="is_range_valid" dataDxfId="13">
+      <calculatedColumnFormula array="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{BB7585E7-7A1E-4252-AA6B-D26E6E875178}" name="range_type" dataDxfId="12">
+      <calculatedColumnFormula>IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="9" xr3:uid="{BED36B27-E0F9-4923-B084-ABAE4CD0BE78}" name="sql_data_type" dataDxfId="11">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
@@ -738,13 +861,15 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -755,25 +880,34 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -792,12 +926,24 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="str">
+      <c r="I2" s="5" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v/>
+      </c>
+      <c r="J2" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J2" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v/>
+      </c>
+      <c r="K2" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v/>
+      </c>
+      <c r="L2" s="5" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>VARCHAR</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -816,12 +962,24 @@
       <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" t="str">
+      <c r="I3" s="5" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v/>
+      </c>
+      <c r="J3" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J3" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v/>
+      </c>
+      <c r="K3" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v/>
+      </c>
+      <c r="L3" s="5" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>VARCHAR</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -840,12 +998,24 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="str">
+      <c r="I4" s="5" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v/>
+      </c>
+      <c r="J4" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J4" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v/>
+      </c>
+      <c r="K4" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v/>
+      </c>
+      <c r="L4" s="5" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>INT</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -864,12 +1034,24 @@
       <c r="H5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" t="str">
+      <c r="I5" s="5" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v/>
+      </c>
+      <c r="J5" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J5" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v/>
+      </c>
+      <c r="K5" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v/>
+      </c>
+      <c r="L5" s="5" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>FLOAT</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -888,47 +1070,71 @@
       <c r="H6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" t="str">
+      <c r="I6" s="5" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v/>
+      </c>
+      <c r="J6" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J6" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v/>
+      </c>
+      <c r="K6" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v/>
+      </c>
+      <c r="L6" s="5" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>DATETIME</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
       </c>
       <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
         <v>52</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="3" t="str">
+      <c r="I7" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>A2:A51</v>
+      </c>
+      <c r="J7" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J7" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K7" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L7" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>INT</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -937,79 +1143,115 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="3" t="str">
+      <c r="I8" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>B2:B51</v>
+      </c>
+      <c r="J8" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J8" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K8" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L8" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>INT</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="3" t="str">
+      <c r="I9" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>C2:C51</v>
+      </c>
+      <c r="J9" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J9" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K9" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L9" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>FLOAT</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="3" t="str">
+      <c r="I10" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>D2:D51</v>
+      </c>
+      <c r="J10" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J10" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K10" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L10" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>FLOAT</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
         <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -1018,25 +1260,37 @@
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="3" t="str">
+      <c r="I11" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>B1:AY1</v>
+      </c>
+      <c r="J11" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J11" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same row</v>
+      </c>
+      <c r="K11" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>row</v>
+      </c>
+      <c r="L11" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>DATETIME</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -1045,25 +1299,37 @@
         <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="3" t="str">
+      <c r="I12" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>B2:AY2</v>
+      </c>
+      <c r="J12" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J12" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same row</v>
+      </c>
+      <c r="K12" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>row</v>
+      </c>
+      <c r="L12" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>INT</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
@@ -1072,25 +1338,37 @@
         <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="3" t="str">
+      <c r="I13" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>B3:AY3</v>
+      </c>
+      <c r="J13" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J13" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same row</v>
+      </c>
+      <c r="K13" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>row</v>
+      </c>
+      <c r="L13" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>INT</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -1099,25 +1377,37 @@
         <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="3" t="str">
+      <c r="I14" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>B4:AY4</v>
+      </c>
+      <c r="J14" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J14" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same row</v>
+      </c>
+      <c r="K14" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>row</v>
+      </c>
+      <c r="L14" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>FLOAT</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -1126,18 +1416,38 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="3" t="str">
+      <c r="I15" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <v>B5:AY5</v>
+      </c>
+      <c r="J15" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J15" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same row</v>
+      </c>
+      <c r="K15" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>row</v>
+      </c>
+      <c r="L15" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>FLOAT</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="J2:K15">
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="INVALID">
+      <formula>NOT(ISERROR(SEARCH("INVALID",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+  </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H15" xr:uid="{B8EBBD32-1EB1-4524-B24A-2106857AC088}">
       <formula1>pandas_data_types</formula1>
@@ -1161,25 +1471,16 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="20.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>75</v>
+      <c r="A1" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -1206,9 +1507,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="105.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>76</v>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
@@ -1226,24 +1527,24 @@
         <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>77</v>
+      <c r="A3" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1265,9 +1566,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Logic fixed, basics tested and working
</commit_message>
<xml_diff>
--- a/scrape_targets.xlsx
+++ b/scrape_targets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\PythonProjects\ExcelExtractorPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2FF86C-5AD3-4D43-8770-E7B7AC4F8944}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415D1A3E-AC54-4F9A-92D1-58BA6FF07A97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15460" xr2:uid="{518FEAFD-939C-4A7D-A483-F0BB88014974}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15460" xr2:uid="{518FEAFD-939C-4A7D-A483-F0BB88014974}"/>
   </bookViews>
   <sheets>
     <sheet name="target_data" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="83">
   <si>
     <t>sql_table</t>
   </si>
@@ -281,12 +281,6 @@
     <t>is_target_a_cell_or_range_of_cells</t>
   </si>
   <si>
-    <t>range_data_start</t>
-  </si>
-  <si>
-    <t>range_data_end</t>
-  </si>
-  <si>
     <t>Column Name:</t>
   </si>
   <si>
@@ -297,9 +291,6 @@
   </si>
   <si>
     <t>Try to keep cells to their own tables and ranges to their own tables. If you have a table where one column is 'Country Name' and it = 'England' and you try to include a range in the same table, say 'Year' which runs from 1900 to 2000, then you will end up with the 'Country Name' column containing 100x instances of 'England'. This is very data inefficient and if you begin working with hundreds or thousands of mixed cell/range tables then you will soon get into millions of rows/columns of data where there should only be thousands (think: GB of data vs MB or even KB)</t>
-  </si>
-  <si>
-    <t>range_target</t>
   </si>
   <si>
     <t>The starting cell IF AND ONLY IF the target is a range. Range start/end must be same row/column.
@@ -314,6 +305,18 @@
   </si>
   <si>
     <t>range_type</t>
+  </si>
+  <si>
+    <t>target_cell</t>
+  </si>
+  <si>
+    <t>target_range</t>
+  </si>
+  <si>
+    <t>target_range_start</t>
+  </si>
+  <si>
+    <t>target_range_end</t>
   </si>
 </sst>
 </file>
@@ -522,15 +525,15 @@
     <tableColumn id="2" xr3:uid="{F7A916CE-56BF-450D-8D09-4C0D3640E4FB}" name="sql_table"/>
     <tableColumn id="3" xr3:uid="{5E08581E-A626-41E4-A3A6-E7092DE71F3F}" name="column_name"/>
     <tableColumn id="4" xr3:uid="{E3D9983E-E54B-4F32-A9BF-A27EB1329ADE}" name="is_target_a_cell_or_range_of_cells"/>
-    <tableColumn id="5" xr3:uid="{3D4629AB-F2BC-47C5-8349-7E109F964BFA}" name="cell_position"/>
-    <tableColumn id="6" xr3:uid="{54F89EEC-33E3-407A-A390-2297247EA74B}" name="range_data_start"/>
-    <tableColumn id="7" xr3:uid="{F060C16F-F16D-4308-A0EB-522EA932101E}" name="range_data_end"/>
+    <tableColumn id="5" xr3:uid="{3D4629AB-F2BC-47C5-8349-7E109F964BFA}" name="target_cell"/>
+    <tableColumn id="6" xr3:uid="{54F89EEC-33E3-407A-A390-2297247EA74B}" name="target_range_start"/>
+    <tableColumn id="7" xr3:uid="{F060C16F-F16D-4308-A0EB-522EA932101E}" name="target_range_end"/>
     <tableColumn id="13" xr3:uid="{F5983EFB-EE48-4D35-9D9F-1E17636F31B3}" name="pandas_data_type"/>
-    <tableColumn id="10" xr3:uid="{565D067D-9EC2-44EE-B453-12007052D0AC}" name="range_target" dataDxfId="14">
-      <calculatedColumnFormula>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{565D067D-9EC2-44EE-B453-12007052D0AC}" name="target_range" dataDxfId="14">
+      <calculatedColumnFormula>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{262BC145-114C-40E5-A310-C6C9AB7BE343}" name="is_range_valid" dataDxfId="13">
-      <calculatedColumnFormula array="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</calculatedColumnFormula>
+      <calculatedColumnFormula array="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{BB7585E7-7A1E-4252-AA6B-D26E6E875178}" name="range_type" dataDxfId="12">
       <calculatedColumnFormula>IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</calculatedColumnFormula>
@@ -863,9 +866,7 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -883,25 +884,25 @@
         <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>45</v>
@@ -927,11 +928,11 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v/>
       </c>
       <c r="J2" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J2" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J2" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v/>
       </c>
       <c r="K2" s="6" t="str">
@@ -963,11 +964,11 @@
         <v>6</v>
       </c>
       <c r="I3" s="5" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v/>
       </c>
       <c r="J3" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J3" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J3" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v/>
       </c>
       <c r="K3" s="6" t="str">
@@ -999,11 +1000,11 @@
         <v>26</v>
       </c>
       <c r="I4" s="5" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v/>
       </c>
       <c r="J4" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J4" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J4" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v/>
       </c>
       <c r="K4" s="6" t="str">
@@ -1035,11 +1036,11 @@
         <v>27</v>
       </c>
       <c r="I5" s="5" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v/>
       </c>
       <c r="J5" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J5" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J5" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v/>
       </c>
       <c r="K5" s="6" t="str">
@@ -1071,11 +1072,11 @@
         <v>29</v>
       </c>
       <c r="I6" s="5" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v/>
       </c>
       <c r="J6" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J6" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J6" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v/>
       </c>
       <c r="K6" s="6" t="str">
@@ -1110,11 +1111,11 @@
         <v>26</v>
       </c>
       <c r="I7" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>A2:A51</v>
       </c>
       <c r="J7" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J7" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J7" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same column</v>
       </c>
       <c r="K7" s="6" t="str">
@@ -1149,11 +1150,11 @@
         <v>26</v>
       </c>
       <c r="I8" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>B2:B51</v>
       </c>
       <c r="J8" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J8" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J8" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same column</v>
       </c>
       <c r="K8" s="6" t="str">
@@ -1188,11 +1189,11 @@
         <v>27</v>
       </c>
       <c r="I9" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>C2:C51</v>
       </c>
       <c r="J9" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J9" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J9" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same column</v>
       </c>
       <c r="K9" s="6" t="str">
@@ -1227,11 +1228,11 @@
         <v>27</v>
       </c>
       <c r="I10" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>D2:D51</v>
       </c>
       <c r="J10" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J10" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J10" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same column</v>
       </c>
       <c r="K10" s="6" t="str">
@@ -1266,11 +1267,11 @@
         <v>29</v>
       </c>
       <c r="I11" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>B1:AY1</v>
       </c>
       <c r="J11" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J11" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J11" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same row</v>
       </c>
       <c r="K11" s="6" t="str">
@@ -1305,11 +1306,11 @@
         <v>26</v>
       </c>
       <c r="I12" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>B2:AY2</v>
       </c>
       <c r="J12" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J12" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J12" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same row</v>
       </c>
       <c r="K12" s="6" t="str">
@@ -1344,11 +1345,11 @@
         <v>26</v>
       </c>
       <c r="I13" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>B3:AY3</v>
       </c>
       <c r="J13" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J13" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J13" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same row</v>
       </c>
       <c r="K13" s="6" t="str">
@@ -1383,11 +1384,11 @@
         <v>27</v>
       </c>
       <c r="I14" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>B4:AY4</v>
       </c>
       <c r="J14" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J14" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J14" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same row</v>
       </c>
       <c r="K14" s="6" t="str">
@@ -1422,11 +1423,11 @@
         <v>27</v>
       </c>
       <c r="I15" s="6" t="str">
-        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[range_data_start]],":",Table1[[#This Row],[range_data_end]]),"")</f>
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
         <v>B5:AY5</v>
       </c>
       <c r="J15" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="J15" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[range_data_start]]))=ROW(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[range_data_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[range_data_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <f t="array" aca="1" ref="J15" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
         <v>yes - same row</v>
       </c>
       <c r="K15" s="6" t="str">
@@ -1480,7 +1481,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -1509,7 +1510,7 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
@@ -1527,7 +1528,7 @@
         <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>42</v>
@@ -1538,13 +1539,13 @@
     </row>
     <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>

</xml_diff>

<commit_message>
Increased efficiency of column iteration
</commit_message>
<xml_diff>
--- a/scrape_targets.xlsx
+++ b/scrape_targets.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\PythonProjects\ExcelExtractorPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51B9A77-C483-47BA-8C3D-0A1AC282C3B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C868EA-F1E6-4D60-81C1-7B98A5160F10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-230" windowWidth="38620" windowHeight="21220" xr2:uid="{518FEAFD-939C-4A7D-A483-F0BB88014974}"/>
   </bookViews>
   <sheets>
     <sheet name="target_data" sheetId="1" r:id="rId1"/>
-    <sheet name="target_data_explained" sheetId="3" r:id="rId2"/>
-    <sheet name="dropdowns" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="target_data_explained" sheetId="3" r:id="rId4"/>
+    <sheet name="dropdowns" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="is_target_cell_or_range">dropdowns!$C$2:$C$3</definedName>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="130">
   <si>
     <t>sql_table</t>
   </si>
@@ -77,9 +79,6 @@
     <t>cell_position</t>
   </si>
   <si>
-    <t>B1</t>
-  </si>
-  <si>
     <t>VARCHAR</t>
   </si>
   <si>
@@ -101,39 +100,6 @@
     <t>source_sheet</t>
   </si>
   <si>
-    <t>Country Template</t>
-  </si>
-  <si>
-    <t>countries_stats</t>
-  </si>
-  <si>
-    <t>country_name</t>
-  </si>
-  <si>
-    <t>country_capital</t>
-  </si>
-  <si>
-    <t>country_pop</t>
-  </si>
-  <si>
-    <t>country_unemp_pc</t>
-  </si>
-  <si>
-    <t>country_unemp_pc_date</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>B3</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
@@ -203,79 +169,10 @@
     <t>sql_data_type</t>
   </si>
   <si>
-    <t>Figures</t>
-  </si>
-  <si>
-    <t>country_lf_year</t>
-  </si>
-  <si>
-    <t>country_lf_year_num</t>
-  </si>
-  <si>
-    <t>country_lf_gdp</t>
-  </si>
-  <si>
-    <t>country_lf_int_rate</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A51</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
     <t>D2</t>
-  </si>
-  <si>
-    <t>B51</t>
-  </si>
-  <si>
-    <t>C51</t>
-  </si>
-  <si>
-    <t>D51</t>
-  </si>
-  <si>
-    <t>Historic Figures</t>
-  </si>
-  <si>
-    <t>countries_figs_live</t>
-  </si>
-  <si>
-    <t>countries_figs_hist</t>
-  </si>
-  <si>
-    <t>country_hf_date</t>
-  </si>
-  <si>
-    <t>country_hf_year</t>
-  </si>
-  <si>
-    <t>country_hf_year_num</t>
-  </si>
-  <si>
-    <t>country_hf_gdp</t>
-  </si>
-  <si>
-    <t>country_hf_int_rate</t>
-  </si>
-  <si>
-    <t>AY1</t>
-  </si>
-  <si>
-    <t>AY2</t>
-  </si>
-  <si>
-    <t>AY3</t>
-  </si>
-  <si>
-    <t>AY4</t>
-  </si>
-  <si>
-    <t>AY5</t>
   </si>
   <si>
     <t>is_target_a_cell_or_range_of_cells</t>
@@ -317,6 +214,252 @@
   </si>
   <si>
     <t>target_range_end</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>sheet_rows</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>col_thing1</t>
+  </si>
+  <si>
+    <t>col_thing2</t>
+  </si>
+  <si>
+    <t>col_thing3</t>
+  </si>
+  <si>
+    <t>col_thing4</t>
+  </si>
+  <si>
+    <t>col_thing5</t>
+  </si>
+  <si>
+    <t>col_thing6</t>
+  </si>
+  <si>
+    <t>col_thing7</t>
+  </si>
+  <si>
+    <t>col_thing8</t>
+  </si>
+  <si>
+    <t>col_thing9</t>
+  </si>
+  <si>
+    <t>col_thing10</t>
+  </si>
+  <si>
+    <t>col_thing11</t>
+  </si>
+  <si>
+    <t>col_thing12</t>
+  </si>
+  <si>
+    <t>row_thing1</t>
+  </si>
+  <si>
+    <t>row_thing2</t>
+  </si>
+  <si>
+    <t>row_thing3</t>
+  </si>
+  <si>
+    <t>row_thing4</t>
+  </si>
+  <si>
+    <t>row_thing5</t>
+  </si>
+  <si>
+    <t>row_thing6</t>
+  </si>
+  <si>
+    <t>row_thing7</t>
+  </si>
+  <si>
+    <t>row_thing8</t>
+  </si>
+  <si>
+    <t>row_thing9</t>
+  </si>
+  <si>
+    <t>row_thing10</t>
+  </si>
+  <si>
+    <t>row_thing11</t>
+  </si>
+  <si>
+    <t>row_thing12</t>
+  </si>
+  <si>
+    <t>cols</t>
+  </si>
+  <si>
+    <t>sheet_cols</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A401</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>B401</t>
+  </si>
+  <si>
+    <t>C401</t>
+  </si>
+  <si>
+    <t>D401</t>
+  </si>
+  <si>
+    <t>E401</t>
+  </si>
+  <si>
+    <t>F401</t>
+  </si>
+  <si>
+    <t>G401</t>
+  </si>
+  <si>
+    <t>H401</t>
+  </si>
+  <si>
+    <t>I401</t>
+  </si>
+  <si>
+    <t>J401</t>
+  </si>
+  <si>
+    <t>K401</t>
+  </si>
+  <si>
+    <t>A50</t>
+  </si>
+  <si>
+    <t>B50</t>
+  </si>
+  <si>
+    <t>C50</t>
+  </si>
+  <si>
+    <t>D50</t>
+  </si>
+  <si>
+    <t>E50</t>
+  </si>
+  <si>
+    <t>F50</t>
+  </si>
+  <si>
+    <t>G50</t>
+  </si>
+  <si>
+    <t>H50</t>
+  </si>
+  <si>
+    <t>I50</t>
+  </si>
+  <si>
+    <t>J50</t>
+  </si>
+  <si>
+    <t>K50</t>
+  </si>
+  <si>
+    <t>AX1</t>
+  </si>
+  <si>
+    <t>AX2</t>
+  </si>
+  <si>
+    <t>AX3</t>
+  </si>
+  <si>
+    <t>AX4</t>
+  </si>
+  <si>
+    <t>AX5</t>
+  </si>
+  <si>
+    <t>AX6</t>
+  </si>
+  <si>
+    <t>AX7</t>
+  </si>
+  <si>
+    <t>AX8</t>
+  </si>
+  <si>
+    <t>AX9</t>
+  </si>
+  <si>
+    <t>AX10</t>
+  </si>
+  <si>
+    <t>AX11</t>
+  </si>
+  <si>
+    <t>AX12</t>
   </si>
 </sst>
 </file>
@@ -346,7 +489,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,8 +502,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -368,11 +517,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -388,31 +552,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -451,6 +597,16 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -504,6 +660,26 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -518,8 +694,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{463491B0-F0FB-4A54-A8DF-FE4522A53DC6}" name="Table1" displayName="Table1" ref="A1:L15" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:L15" xr:uid="{1CBFAB26-4B89-4259-9A52-23CEBACB033B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{463491B0-F0FB-4A54-A8DF-FE4522A53DC6}" name="Table1" displayName="Table1" ref="A1:L25" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:L25" xr:uid="{1CBFAB26-4B89-4259-9A52-23CEBACB033B}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{A93C40C7-C2F4-4A55-81DC-2E3E4884ACA4}" name="source_sheet"/>
     <tableColumn id="2" xr3:uid="{F7A916CE-56BF-450D-8D09-4C0D3640E4FB}" name="sql_table"/>
@@ -529,16 +705,16 @@
     <tableColumn id="6" xr3:uid="{54F89EEC-33E3-407A-A390-2297247EA74B}" name="target_range_start"/>
     <tableColumn id="7" xr3:uid="{F060C16F-F16D-4308-A0EB-522EA932101E}" name="target_range_end"/>
     <tableColumn id="13" xr3:uid="{F5983EFB-EE48-4D35-9D9F-1E17636F31B3}" name="pandas_data_type"/>
-    <tableColumn id="10" xr3:uid="{565D067D-9EC2-44EE-B453-12007052D0AC}" name="target_range" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{565D067D-9EC2-44EE-B453-12007052D0AC}" name="target_range" dataDxfId="15">
       <calculatedColumnFormula>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{262BC145-114C-40E5-A310-C6C9AB7BE343}" name="is_range_valid" dataDxfId="15">
+    <tableColumn id="11" xr3:uid="{262BC145-114C-40E5-A310-C6C9AB7BE343}" name="is_range_valid" dataDxfId="14">
       <calculatedColumnFormula array="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB7585E7-7A1E-4252-AA6B-D26E6E875178}" name="range_type" dataDxfId="14">
+    <tableColumn id="12" xr3:uid="{BB7585E7-7A1E-4252-AA6B-D26E6E875178}" name="range_type" dataDxfId="13">
       <calculatedColumnFormula>IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{BED36B27-E0F9-4923-B084-ABAE4CD0BE78}" name="sql_data_type" dataDxfId="13">
+    <tableColumn id="9" xr3:uid="{BED36B27-E0F9-4923-B084-ABAE4CD0BE78}" name="sql_data_type" dataDxfId="12">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -547,18 +723,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6DA8898D-2440-4B38-9D6F-270BCC333A09}" name="Table14" displayName="Table14" ref="A1:I3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6DA8898D-2440-4B38-9D6F-270BCC333A09}" name="Table14" displayName="Table14" ref="A1:I3" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I3" xr:uid="{F4CE9BD4-6AF0-4706-926F-73D72B4AED87}"/>
   <tableColumns count="9">
-    <tableColumn id="10" xr3:uid="{16A9238A-7273-426F-BA0A-63D65111F5AB}" name="Column Name:" dataDxfId="10"/>
-    <tableColumn id="1" xr3:uid="{DD34C9AB-37EC-4A87-B81F-3817399BA0B6}" name="source_sheet" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{A82271DE-EAEE-4809-9384-22B8DDA8F2C5}" name="sql_table" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{0D585A85-E0A8-45F1-A20C-81CD7492AF5A}" name="column_name" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{E21C8092-DDA8-499C-B514-74BA8F80BD88}" name="cell_or_range" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{5DF34191-0074-479E-9DD3-59ECF34F700E}" name="cell_position" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4C52C704-FBB5-4ACD-90ED-C5AE28D00D4B}" name="range_start" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{6FD1D3B0-53B5-491F-B2DB-3442AD8000D2}" name="range_end" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{93E92658-BB13-4E8D-A8D1-80B37BD475F0}" name="data_type" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{16A9238A-7273-426F-BA0A-63D65111F5AB}" name="Column Name:" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{DD34C9AB-37EC-4A87-B81F-3817399BA0B6}" name="source_sheet" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A82271DE-EAEE-4809-9384-22B8DDA8F2C5}" name="sql_table" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{0D585A85-E0A8-45F1-A20C-81CD7492AF5A}" name="column_name" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{E21C8092-DDA8-499C-B514-74BA8F80BD88}" name="cell_or_range" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5DF34191-0074-479E-9DD3-59ECF34F700E}" name="cell_position" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{4C52C704-FBB5-4ACD-90ED-C5AE28D00D4B}" name="range_start" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{6FD1D3B0-53B5-491F-B2DB-3442AD8000D2}" name="range_end" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{93E92658-BB13-4E8D-A8D1-80B37BD475F0}" name="data_type" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -864,17 +1040,17 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -883,246 +1059,261 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>118</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I2" s="5" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v/>
+        <v>B1:AX1</v>
       </c>
       <c r="J2" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v/>
+        <v>yes - same row</v>
       </c>
       <c r="K2" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v/>
+        <v>row</v>
       </c>
       <c r="L2" s="5" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>VARCHAR</v>
+        <v>INT</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" t="s">
+        <v>119</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="5" t="str">
+        <v>14</v>
+      </c>
+      <c r="I3" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v/>
+        <v>B2:AX2</v>
       </c>
       <c r="J3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v/>
+        <v>yes - same row</v>
       </c>
       <c r="K3" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v/>
-      </c>
-      <c r="L3" s="5" t="str">
+        <v>row</v>
+      </c>
+      <c r="L3" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>VARCHAR</v>
+        <v>INT</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>120</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="5" t="str">
+        <v>14</v>
+      </c>
+      <c r="I4" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v/>
+        <v>B3:AX3</v>
       </c>
       <c r="J4" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v/>
+        <v>yes - same row</v>
       </c>
       <c r="K4" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v/>
-      </c>
-      <c r="L4" s="5" t="str">
+        <v>row</v>
+      </c>
+      <c r="L4" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
         <v>INT</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>121</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="5" t="str">
+        <v>14</v>
+      </c>
+      <c r="I5" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v/>
+        <v>B4:AX4</v>
       </c>
       <c r="J5" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v/>
+        <v>yes - same row</v>
       </c>
       <c r="K5" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v/>
-      </c>
-      <c r="L5" s="5" t="str">
+        <v>row</v>
+      </c>
+      <c r="L5" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>FLOAT</v>
+        <v>INT</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="5" t="str">
+        <v>14</v>
+      </c>
+      <c r="I6" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v/>
+        <v>B5:AX5</v>
       </c>
       <c r="J6" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v/>
+        <v>yes - same row</v>
       </c>
       <c r="K6" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v/>
-      </c>
-      <c r="L6" s="5" t="str">
+        <v>row</v>
+      </c>
+      <c r="L6" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>DATETIME</v>
+        <v>INT</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="I7" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>A2:A51</v>
+        <v>B6:AX6</v>
       </c>
       <c r="J7" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v>yes - same column</v>
+        <v>yes - same row</v>
       </c>
       <c r="K7" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v>column</v>
+        <v>row</v>
       </c>
       <c r="L7" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
@@ -1131,37 +1322,37 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="G8" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="I8" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B2:B51</v>
+        <v>B7:AX7</v>
       </c>
       <c r="J8" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v>yes - same column</v>
+        <v>yes - same row</v>
       </c>
       <c r="K8" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v>column</v>
+        <v>row</v>
       </c>
       <c r="L8" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
@@ -1170,107 +1361,107 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I9" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>C2:C51</v>
+        <v>B8:AX8</v>
       </c>
       <c r="J9" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v>yes - same column</v>
+        <v>yes - same row</v>
       </c>
       <c r="K9" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v>column</v>
+        <v>row</v>
       </c>
       <c r="L9" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>FLOAT</v>
+        <v>INT</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I10" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>D2:D51</v>
+        <v>B9:AX9</v>
       </c>
       <c r="J10" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v>yes - same column</v>
+        <v>yes - same row</v>
       </c>
       <c r="K10" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v>column</v>
+        <v>row</v>
       </c>
       <c r="L10" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>FLOAT</v>
+        <v>INT</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="I11" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B1:AY1</v>
+        <v>B10:AX10</v>
       </c>
       <c r="J11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1282,34 +1473,34 @@
       </c>
       <c r="L11" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>DATETIME</v>
+        <v>INT</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="I12" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B2:AY2</v>
+        <v>B11:AX11</v>
       </c>
       <c r="J12" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1326,29 +1517,29 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="I13" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B3:AY3</v>
+        <v>B12:AX12</v>
       </c>
       <c r="J13" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1365,97 +1556,487 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I14" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B4:AY4</v>
+        <v>A2:A50</v>
       </c>
       <c r="J14" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v>yes - same row</v>
+        <v>yes - same column</v>
       </c>
       <c r="K14" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v>row</v>
+        <v>column</v>
       </c>
       <c r="L14" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>FLOAT</v>
+        <v>INT</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
       <c r="H15" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I15" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B5:AY5</v>
+        <v>A2:A50</v>
       </c>
       <c r="J15" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J15" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
-        <v>yes - same row</v>
+        <v>yes - same column</v>
       </c>
       <c r="K15" s="6" t="str">
         <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
-        <v>row</v>
+        <v>column</v>
       </c>
       <c r="L15" s="6" t="str">
         <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
-        <v>FLOAT</v>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>B2:B50</v>
+      </c>
+      <c r="J16" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J16" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K16" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L16" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>C2:C50</v>
+      </c>
+      <c r="J17" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J17" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K17" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L17" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>D2:D50</v>
+      </c>
+      <c r="J18" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J18" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K18" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L18" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>E2:E50</v>
+      </c>
+      <c r="J19" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J19" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K19" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L19" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>F2:F50</v>
+      </c>
+      <c r="J20" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J20" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K20" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L20" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>G2:G50</v>
+      </c>
+      <c r="J21" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J21" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K21" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L21" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>H2:H50</v>
+      </c>
+      <c r="J22" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J22" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K22" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L22" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>I2:I50</v>
+      </c>
+      <c r="J23" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J23" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K23" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L23" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>J2:J50</v>
+      </c>
+      <c r="J24" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J24" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K24" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L24" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="6" t="str">
+        <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
+        <v>K2:K50</v>
+      </c>
+      <c r="J25" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="J25" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
+        <v>yes - same column</v>
+      </c>
+      <c r="K25" s="6" t="str">
+        <f ca="1">IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="n","column",IF(RIGHT(Table1[[#This Row],[is_range_valid]],1)="w","row",""))</f>
+        <v>column</v>
+      </c>
+      <c r="L25" s="6" t="str">
+        <f>VLOOKUP(Table1[[#This Row],[pandas_data_type]],dropdowns!$A:$B,2,FALSE)</f>
+        <v>INT</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="J2:K15">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="INVALID">
+  <conditionalFormatting sqref="J2:K25">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="INVALID">
       <formula>NOT(ISERROR(SEARCH("INVALID",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H15" xr:uid="{B8EBBD32-1EB1-4524-B24A-2106857AC088}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H25" xr:uid="{5FC4DFDE-BD44-4068-A539-FE8DD52FCFE1}">
       <formula1>pandas_data_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15" xr:uid="{8BB07F2B-3D92-455D-8DBB-2781E1FDE3F1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D25" xr:uid="{F2253F9A-3FA8-4980-A666-8A190D50DC25}">
       <formula1>is_target_cell_or_range</formula1>
     </dataValidation>
   </dataValidations>
@@ -1468,6 +2049,334 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD6DAF9-9B38-48EA-91D6-BB25BB7D3FA8}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C12">
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D12" xr:uid="{7F3CC76E-E574-4EED-89E2-0C6F05EE0C5F}">
+      <formula1>is_target_cell_or_range</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H12" xr:uid="{E35AA9D5-7EC7-40EB-840E-3A40F8AD7B9B}">
+      <formula1>pandas_data_types</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B1A069-4F95-414B-A7AE-5B14768F0691}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E63BE89-4535-4EED-A872-DA3B807C9EE5}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -1483,10 +2392,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1495,16 +2404,16 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -1512,42 +2421,42 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1562,7 +2471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEE643B-A25E-4E34-A909-2EBD9639882C}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
@@ -1580,67 +2489,67 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working V0.9, try-excepts outstanding
</commit_message>
<xml_diff>
--- a/scrape_targets.xlsx
+++ b/scrape_targets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\PythonProjects\ExcelExtractorPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C868EA-F1E6-4D60-81C1-7B98A5160F10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CA55FD-0DCB-4AED-922A-38A3473790FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-230" windowWidth="38620" windowHeight="21220" xr2:uid="{518FEAFD-939C-4A7D-A483-F0BB88014974}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{518FEAFD-939C-4A7D-A483-F0BB88014974}"/>
   </bookViews>
   <sheets>
     <sheet name="target_data" sheetId="1" r:id="rId1"/>
@@ -393,73 +393,73 @@
     <t>K401</t>
   </si>
   <si>
-    <t>A50</t>
-  </si>
-  <si>
-    <t>B50</t>
-  </si>
-  <si>
-    <t>C50</t>
-  </si>
-  <si>
-    <t>D50</t>
-  </si>
-  <si>
-    <t>E50</t>
-  </si>
-  <si>
-    <t>F50</t>
-  </si>
-  <si>
-    <t>G50</t>
-  </si>
-  <si>
-    <t>H50</t>
-  </si>
-  <si>
-    <t>I50</t>
-  </si>
-  <si>
-    <t>J50</t>
-  </si>
-  <si>
-    <t>K50</t>
-  </si>
-  <si>
-    <t>AX1</t>
-  </si>
-  <si>
-    <t>AX2</t>
-  </si>
-  <si>
-    <t>AX3</t>
-  </si>
-  <si>
-    <t>AX4</t>
-  </si>
-  <si>
-    <t>AX5</t>
-  </si>
-  <si>
-    <t>AX6</t>
-  </si>
-  <si>
-    <t>AX7</t>
-  </si>
-  <si>
-    <t>AX8</t>
-  </si>
-  <si>
-    <t>AX9</t>
-  </si>
-  <si>
-    <t>AX10</t>
-  </si>
-  <si>
-    <t>AX11</t>
-  </si>
-  <si>
-    <t>AX12</t>
+    <t>XFD1</t>
+  </si>
+  <si>
+    <t>XFD2</t>
+  </si>
+  <si>
+    <t>XFD3</t>
+  </si>
+  <si>
+    <t>XFD4</t>
+  </si>
+  <si>
+    <t>XFD5</t>
+  </si>
+  <si>
+    <t>XFD6</t>
+  </si>
+  <si>
+    <t>XFD7</t>
+  </si>
+  <si>
+    <t>XFD8</t>
+  </si>
+  <si>
+    <t>XFD9</t>
+  </si>
+  <si>
+    <t>XFD10</t>
+  </si>
+  <si>
+    <t>XFD11</t>
+  </si>
+  <si>
+    <t>XFD12</t>
+  </si>
+  <si>
+    <t>A163840</t>
+  </si>
+  <si>
+    <t>B163840</t>
+  </si>
+  <si>
+    <t>C163840</t>
+  </si>
+  <si>
+    <t>D163840</t>
+  </si>
+  <si>
+    <t>E163840</t>
+  </si>
+  <si>
+    <t>F163840</t>
+  </si>
+  <si>
+    <t>G163840</t>
+  </si>
+  <si>
+    <t>H163840</t>
+  </si>
+  <si>
+    <t>I163840</t>
+  </si>
+  <si>
+    <t>J163840</t>
+  </si>
+  <si>
+    <t>K163840</t>
   </si>
 </sst>
 </file>
@@ -1042,9 +1042,7 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1103,14 +1101,14 @@
         <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="5" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B1:AX1</v>
+        <v>B1:XFD1</v>
       </c>
       <c r="J2" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1142,14 +1140,14 @@
         <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B2:AX2</v>
+        <v>B2:XFD2</v>
       </c>
       <c r="J3" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1181,14 +1179,14 @@
         <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B3:AX3</v>
+        <v>B3:XFD3</v>
       </c>
       <c r="J4" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1220,14 +1218,14 @@
         <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B4:AX4</v>
+        <v>B4:XFD4</v>
       </c>
       <c r="J5" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1259,14 +1257,14 @@
         <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B5:AX5</v>
+        <v>B5:XFD5</v>
       </c>
       <c r="J6" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1298,14 +1296,14 @@
         <v>87</v>
       </c>
       <c r="G7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B6:AX6</v>
+        <v>B6:XFD6</v>
       </c>
       <c r="J7" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1337,14 +1335,14 @@
         <v>88</v>
       </c>
       <c r="G8" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B7:AX7</v>
+        <v>B7:XFD7</v>
       </c>
       <c r="J8" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1376,14 +1374,14 @@
         <v>89</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B8:AX8</v>
+        <v>B8:XFD8</v>
       </c>
       <c r="J9" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1415,14 +1413,14 @@
         <v>90</v>
       </c>
       <c r="G10" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
       </c>
       <c r="I10" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B9:AX9</v>
+        <v>B9:XFD9</v>
       </c>
       <c r="J10" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1454,14 +1452,14 @@
         <v>91</v>
       </c>
       <c r="G11" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H11" t="s">
         <v>14</v>
       </c>
       <c r="I11" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B10:AX10</v>
+        <v>B10:XFD10</v>
       </c>
       <c r="J11" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1493,14 +1491,14 @@
         <v>92</v>
       </c>
       <c r="G12" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
       </c>
       <c r="I12" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B11:AX11</v>
+        <v>B11:XFD11</v>
       </c>
       <c r="J12" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1532,14 +1530,14 @@
         <v>93</v>
       </c>
       <c r="G13" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B12:AX12</v>
+        <v>B12:XFD12</v>
       </c>
       <c r="J13" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1571,14 +1569,14 @@
         <v>94</v>
       </c>
       <c r="G14" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="H14" t="s">
         <v>14</v>
       </c>
       <c r="I14" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>A2:A50</v>
+        <v>A2:A163840</v>
       </c>
       <c r="J14" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1610,14 +1608,14 @@
         <v>94</v>
       </c>
       <c r="G15" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="H15" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>A2:A50</v>
+        <v>A2:A163840</v>
       </c>
       <c r="J15" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J15" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1649,14 +1647,14 @@
         <v>83</v>
       </c>
       <c r="G16" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="H16" t="s">
         <v>14</v>
       </c>
       <c r="I16" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>B2:B50</v>
+        <v>B2:B163840</v>
       </c>
       <c r="J16" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J16" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1688,14 +1686,14 @@
         <v>34</v>
       </c>
       <c r="G17" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
       </c>
       <c r="I17" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>C2:C50</v>
+        <v>C2:C163840</v>
       </c>
       <c r="J17" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J17" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1727,14 +1725,14 @@
         <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
       </c>
       <c r="I18" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>D2:D50</v>
+        <v>D2:D163840</v>
       </c>
       <c r="J18" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1766,14 +1764,14 @@
         <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
       </c>
       <c r="I19" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>E2:E50</v>
+        <v>E2:E163840</v>
       </c>
       <c r="J19" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J19" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1805,14 +1803,14 @@
         <v>49</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
       </c>
       <c r="I20" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>F2:F50</v>
+        <v>F2:F163840</v>
       </c>
       <c r="J20" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J20" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1844,14 +1842,14 @@
         <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
       </c>
       <c r="I21" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>G2:G50</v>
+        <v>G2:G163840</v>
       </c>
       <c r="J21" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J21" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1883,14 +1881,14 @@
         <v>51</v>
       </c>
       <c r="G22" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
       </c>
       <c r="I22" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>H2:H50</v>
+        <v>H2:H163840</v>
       </c>
       <c r="J22" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1922,14 +1920,14 @@
         <v>52</v>
       </c>
       <c r="G23" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="H23" t="s">
         <v>14</v>
       </c>
       <c r="I23" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>I2:I50</v>
+        <v>I2:I163840</v>
       </c>
       <c r="J23" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J23" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -1961,14 +1959,14 @@
         <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="H24" t="s">
         <v>14</v>
       </c>
       <c r="I24" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>J2:J50</v>
+        <v>J2:J163840</v>
       </c>
       <c r="J24" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J24" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>
@@ -2000,14 +1998,14 @@
         <v>96</v>
       </c>
       <c r="G25" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="H25" t="s">
         <v>14</v>
       </c>
       <c r="I25" s="6" t="str">
         <f>IF(Table1[[#This Row],[is_target_a_cell_or_range_of_cells]]="range",_xlfn.CONCAT(Table1[[#This Row],[target_range_start]],":",Table1[[#This Row],[target_range_end]]),"")</f>
-        <v>K2:K50</v>
+        <v>K2:K163840</v>
       </c>
       <c r="J25" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="J25" ca="1">IFERROR(IF(ROW(INDIRECT(Table1[[#This Row],[target_range_start]]))=ROW(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same row",IF(COLUMN(INDIRECT(Table1[[#This Row],[target_range_start]]))=COLUMN(INDIRECT(Table1[[#This Row],[target_range_end]])),"yes - same column","INVALID: Rows/Columns mismatch")),"")</f>

</xml_diff>